<commit_message>
Update files for lab files received
</commit_message>
<xml_diff>
--- a/app/assets/images/full.xlsx
+++ b/app/assets/images/full.xlsx
@@ -1,49 +1,44 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hscic365-my.sharepoint.com/personal/nobr1_hscic_gov_uk/Documents/My documents/Digital transformation of screening/Interim CC/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rebeccagorton/Documents/Screening/Reporting/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="444" documentId="8_{885E7B92-DCD6-4A22-B519-64DB40547532}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9FBB99F4-5ABC-4A1A-94A0-590F5FA90B78}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED79F863-E19A-8846-A07C-A00B8608FF7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="37480" yWindow="1980" windowWidth="20720" windowHeight="13280" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="15" r:id="rId1"/>
-    <sheet name="Automatic matches" sheetId="1" r:id="rId2"/>
-    <sheet name="Automatic partial hits to proce" sheetId="2" r:id="rId3"/>
-    <sheet name="Automatic rejections (errors)" sheetId="4" r:id="rId4"/>
-    <sheet name="Automatic rejections (policy)" sheetId="5" r:id="rId5"/>
-    <sheet name="To process outstanding" sheetId="6" r:id="rId6"/>
-    <sheet name="To query outstanding" sheetId="7" r:id="rId7"/>
-    <sheet name="To check outstanding" sheetId="8" r:id="rId8"/>
-    <sheet name="Rejections outstanding" sheetId="9" r:id="rId9"/>
-    <sheet name="Checked manual matches" sheetId="10" r:id="rId10"/>
-    <sheet name="Checked dummy registrations" sheetId="11" r:id="rId11"/>
-    <sheet name="Checked rejections removed" sheetId="12" r:id="rId12"/>
-    <sheet name="Checked rejected results resolv" sheetId="13" r:id="rId13"/>
-    <sheet name="Exceptions" sheetId="14" r:id="rId14"/>
+    <sheet name="Total Automatic matches" sheetId="1" r:id="rId2"/>
+    <sheet name="Total partial hits" sheetId="2" r:id="rId3"/>
+    <sheet name="Total non-hits" sheetId="16" r:id="rId4"/>
+    <sheet name="Total rejections (errors)" sheetId="4" r:id="rId5"/>
+    <sheet name="Total rejections (policy)" sheetId="5" r:id="rId6"/>
+    <sheet name="To process outstanding" sheetId="6" r:id="rId7"/>
+    <sheet name="To query outstanding" sheetId="7" r:id="rId8"/>
+    <sheet name="To check outstanding" sheetId="8" r:id="rId9"/>
+    <sheet name="Rejections outstanding" sheetId="9" r:id="rId10"/>
+    <sheet name="Checked manual matches" sheetId="10" r:id="rId11"/>
+    <sheet name="Checked dummy registrations" sheetId="11" r:id="rId12"/>
+    <sheet name="Checked rejections removed" sheetId="12" r:id="rId13"/>
+    <sheet name="Checked rejected results resolv" sheetId="13" r:id="rId14"/>
+    <sheet name="Exceptions" sheetId="14" r:id="rId15"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="568" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="603" uniqueCount="94">
   <si>
     <t>Automatic matches</t>
   </si>
   <si>
-    <t>Automatic rejections (errors)</t>
-  </si>
-  <si>
-    <t>Automatic rejections (policy)</t>
-  </si>
-  <si>
     <t>To process outstanding</t>
   </si>
   <si>
@@ -308,13 +303,19 @@
     <t xml:space="preserve">Summary </t>
   </si>
   <si>
-    <t xml:space="preserve">Automativ partial hits to process </t>
-  </si>
-  <si>
     <t>Total partial hits</t>
   </si>
   <si>
     <t>Total non-hits</t>
+  </si>
+  <si>
+    <t>Total non hits</t>
+  </si>
+  <si>
+    <t>Total rejections (errors)</t>
+  </si>
+  <si>
+    <t>Total rejections (policy)</t>
   </si>
 </sst>
 </file>
@@ -1160,79 +1161,79 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72D226AC-D064-4DD9-B6CB-F550C257C948}">
   <dimension ref="A1:Q4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.38671875" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B3" t="s">
+        <v>85</v>
+      </c>
+      <c r="C3" t="s">
+        <v>84</v>
+      </c>
+      <c r="D3" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.4">
-      <c r="A2" t="s">
+      <c r="E3" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.4">
-      <c r="A3" t="s">
-        <v>88</v>
-      </c>
-      <c r="B3" t="s">
-        <v>87</v>
-      </c>
-      <c r="C3" t="s">
-        <v>86</v>
-      </c>
-      <c r="D3" t="s">
-        <v>92</v>
-      </c>
-      <c r="E3" t="s">
-        <v>93</v>
-      </c>
       <c r="F3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="G3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="H3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="I3" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J3" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="K3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="L3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="M3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="N3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="O3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="P3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="Q3" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.4">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>8000</v>
       </c>
@@ -1292,244 +1293,24 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
-  <dimension ref="A1:L7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+  <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView zoomScale="40" zoomScaleNormal="40" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="8.88671875" style="2"/>
-    <col min="3" max="3" width="10.27734375" style="2" customWidth="1"/>
-    <col min="4" max="4" width="13.6640625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="10.27734375" style="2" customWidth="1"/>
-    <col min="6" max="16384" width="8.88671875" style="2"/>
+    <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.4">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="L3" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A4" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4" s="3">
-        <v>34680</v>
-      </c>
-      <c r="D4" s="2">
-        <v>123451</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="J4" s="3">
-        <v>34680</v>
-      </c>
-      <c r="K4" s="2">
-        <v>123451</v>
-      </c>
-      <c r="L4" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A5" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5" s="3">
-        <v>34681</v>
-      </c>
-      <c r="D5" s="2">
-        <v>123452</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="J5" s="3">
-        <v>34681</v>
-      </c>
-      <c r="K5" s="2">
-        <v>123452</v>
-      </c>
-      <c r="L5" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A6" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" s="3">
-        <v>34682</v>
-      </c>
-      <c r="D6" s="2">
-        <v>123453</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="J6" s="3">
-        <v>34682</v>
-      </c>
-      <c r="K6" s="2">
-        <v>123453</v>
-      </c>
-      <c r="L6" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A7" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7" s="3">
-        <v>34683</v>
-      </c>
-      <c r="D7" s="2">
-        <v>123454</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="I7" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="J7" s="3">
-        <v>34683</v>
-      </c>
-      <c r="K7" s="2">
-        <v>123454</v>
-      </c>
-      <c r="L7" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
-  <dimension ref="A1:K6"/>
-  <sheetViews>
-    <sheetView zoomScale="40" zoomScaleNormal="40" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.4"/>
-  <cols>
-    <col min="4" max="4" width="10.77734375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A1" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A2" s="2" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -1542,85 +1323,516 @@
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="G3" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="E3" s="2" t="s">
+      <c r="J3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>52</v>
-      </c>
       <c r="K3" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.4">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>12345</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D4" s="3">
         <v>34680</v>
       </c>
+      <c r="E4" s="2">
+        <v>123451</v>
+      </c>
+      <c r="F4" s="3">
+        <v>44487</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="H4" s="2">
+        <v>0</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" s="2">
+        <v>12346</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="3">
+        <v>34681</v>
+      </c>
+      <c r="E5" s="2">
+        <v>123452</v>
+      </c>
+      <c r="F5" s="3">
+        <v>44488</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="H5" s="2">
+        <v>0</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A6" s="2">
+        <v>12347</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="3">
+        <v>34682</v>
+      </c>
+      <c r="E6" s="2">
+        <v>123453</v>
+      </c>
+      <c r="F6" s="3">
+        <v>44489</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="H6" s="2">
+        <v>0</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A7" s="2">
+        <v>12348</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="3">
+        <v>34683</v>
+      </c>
+      <c r="E7" s="2">
+        <v>123454</v>
+      </c>
+      <c r="F7" s="3">
+        <v>44490</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="H7" s="2">
+        <v>0</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+  <dimension ref="A1:L7"/>
+  <sheetViews>
+    <sheetView zoomScale="40" zoomScaleNormal="40" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="2" width="8.85546875" style="2"/>
+    <col min="3" max="3" width="10.28515625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="10.28515625" style="2" customWidth="1"/>
+    <col min="6" max="16384" width="8.85546875" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="3">
+        <v>34680</v>
+      </c>
+      <c r="D4" s="2">
+        <v>123451</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J4" s="3">
+        <v>34680</v>
+      </c>
+      <c r="K4" s="2">
+        <v>123451</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="3">
+        <v>34681</v>
+      </c>
+      <c r="D5" s="2">
+        <v>123452</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J5" s="3">
+        <v>34681</v>
+      </c>
+      <c r="K5" s="2">
+        <v>123452</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="3">
+        <v>34682</v>
+      </c>
+      <c r="D6" s="2">
+        <v>123453</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J6" s="3">
+        <v>34682</v>
+      </c>
+      <c r="K6" s="2">
+        <v>123453</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="3">
+        <v>34683</v>
+      </c>
+      <c r="D7" s="2">
+        <v>123454</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J7" s="3">
+        <v>34683</v>
+      </c>
+      <c r="K7" s="2">
+        <v>123454</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+  <dimension ref="A1:K6"/>
+  <sheetViews>
+    <sheetView zoomScale="40" zoomScaleNormal="40" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4" s="2">
+        <v>12345</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="3">
+        <v>34680</v>
+      </c>
       <c r="E4" s="3">
         <v>44487</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="G4" s="2">
         <v>0</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.4">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>12346</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D5" s="3">
         <v>34681</v>
@@ -1629,33 +1841,33 @@
         <v>44488</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="G5" s="2">
         <v>0</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.4">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>12347</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D6" s="3">
         <v>34682</v>
@@ -1664,22 +1876,22 @@
         <v>44489</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="G6" s="2">
         <v>0</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -1688,22 +1900,22 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:M6"/>
   <sheetViews>
     <sheetView zoomScale="40" zoomScaleNormal="40" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.4">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -1718,56 +1930,56 @@
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="G3" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="F3" s="2" t="s">
+      <c r="J3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>16</v>
-      </c>
       <c r="K3" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.4">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>12345</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D4" s="3">
         <v>34680</v>
@@ -1779,36 +1991,36 @@
         <v>44487</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H4" s="2">
         <v>0</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.4">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>12346</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D5" s="3">
         <v>34681</v>
@@ -1820,36 +2032,36 @@
         <v>44488</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H5" s="2">
         <v>0</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.4">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>12347</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D6" s="3">
         <v>34682</v>
@@ -1861,25 +2073,25 @@
         <v>44489</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H6" s="2">
         <v>0</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="M6" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -1887,22 +2099,22 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:M6"/>
   <sheetViews>
     <sheetView zoomScale="40" zoomScaleNormal="40" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.4">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -1917,56 +2129,56 @@
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="G3" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="F3" s="2" t="s">
+      <c r="J3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>16</v>
-      </c>
       <c r="K3" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.4">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>12345</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D4" s="3">
         <v>34680</v>
@@ -1978,36 +2190,36 @@
         <v>44487</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H4" s="2">
         <v>0</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.4">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>12346</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D5" s="3">
         <v>34681</v>
@@ -2019,36 +2231,36 @@
         <v>44488</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H5" s="2">
         <v>0</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.4">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>12347</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D6" s="3">
         <v>34682</v>
@@ -2060,25 +2272,25 @@
         <v>44489</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H6" s="2">
         <v>0</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="M6" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -2086,7 +2298,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:K6"/>
   <sheetViews>
@@ -2094,20 +2306,20 @@
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="4" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="4.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="4.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.4">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -2120,50 +2332,50 @@
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="G3" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>15</v>
-      </c>
       <c r="J3" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.4">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>12345</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D4" s="3">
         <v>34680</v>
@@ -2175,30 +2387,30 @@
         <v>44487</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H4" s="2">
         <v>0</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.4">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>12346</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D5" s="3">
         <v>34681</v>
@@ -2210,30 +2422,30 @@
         <v>44488</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H5" s="2">
         <v>0</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.4">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>12347</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D6" s="3">
         <v>34682</v>
@@ -2245,19 +2457,19 @@
         <v>44489</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H6" s="2">
         <v>0</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -2269,62 +2481,62 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I35"/>
   <sheetViews>
-    <sheetView zoomScale="40" zoomScaleNormal="40" workbookViewId="0"/>
+    <sheetView zoomScale="117" zoomScaleNormal="117" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="8.88671875" style="2"/>
-    <col min="3" max="3" width="10.83203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.0546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.88671875" style="2"/>
+    <col min="1" max="2" width="8.85546875" style="2"/>
+    <col min="3" max="3" width="10.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.4">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>14</v>
-      </c>
       <c r="G3" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="I3" s="4"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>12345</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D4" s="2">
         <v>34680</v>
@@ -2336,21 +2548,21 @@
         <v>44487</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H4" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>12346</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D5" s="2">
         <v>34681</v>
@@ -2362,21 +2574,21 @@
         <v>44488</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H5" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>12347</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D6" s="2">
         <v>34682</v>
@@ -2388,21 +2600,21 @@
         <v>44489</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H6" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>12348</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D7" s="2">
         <v>34683</v>
@@ -2414,21 +2626,21 @@
         <v>44490</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H7" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>12349</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D8" s="2">
         <v>34684</v>
@@ -2440,21 +2652,21 @@
         <v>44491</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H8" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>12350</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D9" s="2">
         <v>34685</v>
@@ -2466,21 +2678,21 @@
         <v>44492</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H9" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>12351</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D10" s="2">
         <v>34686</v>
@@ -2492,21 +2704,21 @@
         <v>44493</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H10" s="2">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>12352</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D11" s="2">
         <v>34687</v>
@@ -2518,21 +2730,21 @@
         <v>44494</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H11" s="2">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>12353</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D12" s="2">
         <v>34688</v>
@@ -2544,21 +2756,21 @@
         <v>44495</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H12" s="2">
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>12354</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D13" s="2">
         <v>34689</v>
@@ -2570,21 +2782,21 @@
         <v>44496</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H13" s="2">
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>12355</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D14" s="2">
         <v>34690</v>
@@ -2596,21 +2808,21 @@
         <v>44497</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H14" s="2">
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>12356</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D15" s="2">
         <v>34691</v>
@@ -2622,21 +2834,21 @@
         <v>44498</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H15" s="2">
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>12357</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D16" s="2">
         <v>34692</v>
@@ -2648,21 +2860,21 @@
         <v>44499</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H16" s="2">
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>12358</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D17" s="2">
         <v>34693</v>
@@ -2674,21 +2886,21 @@
         <v>44500</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H17" s="2">
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>12359</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D18" s="2">
         <v>34694</v>
@@ -2700,21 +2912,21 @@
         <v>44501</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H18" s="2">
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
         <v>12360</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D19" s="2">
         <v>34695</v>
@@ -2726,21 +2938,21 @@
         <v>44502</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H19" s="2">
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <v>12361</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D20" s="2">
         <v>34696</v>
@@ -2752,21 +2964,21 @@
         <v>44503</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H20" s="2">
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
         <v>12362</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D21" s="2">
         <v>34697</v>
@@ -2778,21 +2990,21 @@
         <v>44504</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H21" s="2">
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
         <v>12363</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D22" s="2">
         <v>34698</v>
@@ -2804,21 +3016,21 @@
         <v>44505</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H22" s="2">
         <v>9</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
         <v>12364</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D23" s="2">
         <v>34699</v>
@@ -2830,21 +3042,21 @@
         <v>44506</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H23" s="2">
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
         <v>12365</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D24" s="2">
         <v>34700</v>
@@ -2856,21 +3068,21 @@
         <v>44507</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H24" s="2">
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
         <v>12366</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D25" s="2">
         <v>34701</v>
@@ -2882,21 +3094,21 @@
         <v>44508</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H25" s="2">
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
         <v>12367</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D26" s="2">
         <v>34702</v>
@@ -2908,21 +3120,21 @@
         <v>44509</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H26" s="2">
         <v>9</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" s="2">
         <v>12368</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D27" s="2">
         <v>34703</v>
@@ -2934,21 +3146,21 @@
         <v>44510</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H27" s="2">
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" s="2">
         <v>12369</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D28" s="2">
         <v>34704</v>
@@ -2960,21 +3172,21 @@
         <v>44511</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H28" s="2">
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" s="2">
         <v>12370</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D29" s="2">
         <v>34705</v>
@@ -2986,21 +3198,21 @@
         <v>44512</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H29" s="2">
         <v>9</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" s="2">
         <v>12371</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D30" s="2">
         <v>34706</v>
@@ -3012,21 +3224,21 @@
         <v>44513</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H30" s="2">
         <v>9</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" s="2">
         <v>12372</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D31" s="2">
         <v>34707</v>
@@ -3038,21 +3250,21 @@
         <v>44514</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H31" s="2">
         <v>9</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" s="2">
         <v>12373</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D32" s="2">
         <v>34708</v>
@@ -3064,21 +3276,21 @@
         <v>44515</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H32" s="2">
         <v>9</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" s="2">
         <v>12374</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D33" s="2">
         <v>34709</v>
@@ -3090,21 +3302,21 @@
         <v>44516</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H33" s="2">
         <v>9</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" s="2">
         <v>12375</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D34" s="2">
         <v>34710</v>
@@ -3116,21 +3328,21 @@
         <v>44517</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H34" s="2">
         <v>9</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" s="2">
         <v>12376</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D35" s="2">
         <v>34711</v>
@@ -3142,7 +3354,7 @@
         <v>44518</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H35" s="2">
         <v>9</v>
@@ -3157,62 +3369,64 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J9"/>
   <sheetViews>
-    <sheetView zoomScale="40" zoomScaleNormal="40" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="16384" width="8.88671875" style="2"/>
+    <col min="1" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A2" s="2" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="G3" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>15</v>
-      </c>
       <c r="J3" s="4"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>12345</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D4" s="3">
         <v>34680</v>
@@ -3224,24 +3438,24 @@
         <v>44487</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H4" s="2">
         <v>0</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.4">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>12346</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D5" s="3">
         <v>34681</v>
@@ -3253,24 +3467,24 @@
         <v>44488</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H5" s="2">
         <v>0</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.4">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>12347</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D6" s="3">
         <v>34682</v>
@@ -3282,24 +3496,24 @@
         <v>44489</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H6" s="2">
         <v>0</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>12348</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D7" s="3">
         <v>34683</v>
@@ -3311,24 +3525,24 @@
         <v>44490</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H7" s="2">
         <v>0</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.4">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>12349</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D8" s="3">
         <v>34684</v>
@@ -3340,24 +3554,24 @@
         <v>44491</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H8" s="2">
         <v>0</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.4">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>12350</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D9" s="3">
         <v>34685</v>
@@ -3369,13 +3583,13 @@
         <v>44492</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H9" s="2">
         <v>0</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -3385,26 +3599,258 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41AD5E0A-D071-4145-9065-DFB64AD69D2C}">
+  <dimension ref="A1:J9"/>
+  <sheetViews>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="16384" width="8.85546875" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J3" s="4"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" s="2">
+        <v>12345</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="3">
+        <v>34680</v>
+      </c>
+      <c r="E4" s="2">
+        <v>123451</v>
+      </c>
+      <c r="F4" s="3">
+        <v>44487</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="H4" s="2">
+        <v>0</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" s="2">
+        <v>12346</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="3">
+        <v>34681</v>
+      </c>
+      <c r="E5" s="2">
+        <v>123452</v>
+      </c>
+      <c r="F5" s="3">
+        <v>44488</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="H5" s="2">
+        <v>0</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" s="2">
+        <v>12347</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="3">
+        <v>34682</v>
+      </c>
+      <c r="E6" s="2">
+        <v>123453</v>
+      </c>
+      <c r="F6" s="3">
+        <v>44489</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="H6" s="2">
+        <v>0</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7" s="2">
+        <v>12348</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="3">
+        <v>34683</v>
+      </c>
+      <c r="E7" s="2">
+        <v>123454</v>
+      </c>
+      <c r="F7" s="3">
+        <v>44490</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="H7" s="2">
+        <v>0</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" s="2">
+        <v>12349</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="3">
+        <v>34684</v>
+      </c>
+      <c r="E8" s="2">
+        <v>123455</v>
+      </c>
+      <c r="F8" s="3">
+        <v>44491</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="H8" s="2">
+        <v>0</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9" s="2">
+        <v>12350</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" s="3">
+        <v>34685</v>
+      </c>
+      <c r="E9" s="2">
+        <v>123456</v>
+      </c>
+      <c r="F9" s="3">
+        <v>44492</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="H9" s="2">
+        <v>0</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="10" max="10" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.4">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>1</v>
+        <v>92</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -3417,50 +3863,50 @@
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="G3" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="F3" s="2" t="s">
+      <c r="J3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>16</v>
-      </c>
       <c r="K3" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.4">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>12345</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D4" s="3">
         <v>34680</v>
@@ -3472,30 +3918,30 @@
         <v>44487</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H4" s="2">
         <v>0</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.4">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>12346</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D5" s="3">
         <v>34681</v>
@@ -3507,30 +3953,30 @@
         <v>44488</v>
       </c>
       <c r="G5" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="H5" s="2">
+        <v>0</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K5" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="H5" s="2">
-        <v>0</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="J5" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="K5" s="2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.4">
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>12347</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D6" s="3">
         <v>34682</v>
@@ -3542,30 +3988,30 @@
         <v>44489</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H6" s="2">
         <v>0</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.4">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>12348</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D7" s="3">
         <v>34683</v>
@@ -3577,30 +4023,30 @@
         <v>44490</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H7" s="2">
         <v>0</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.4">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>12349</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D8" s="3">
         <v>34684</v>
@@ -3612,30 +4058,30 @@
         <v>44491</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H8" s="2">
         <v>0</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.4">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>12350</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D9" s="3">
         <v>34685</v>
@@ -3647,19 +4093,19 @@
         <v>44492</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H9" s="2">
         <v>0</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -3667,27 +4113,27 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:K7"/>
   <sheetViews>
-    <sheetView zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+    <sheetView zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="10" max="10" width="29.38671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="29.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.4">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>2</v>
+        <v>93</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -3700,50 +4146,50 @@
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="G3" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="F3" s="2" t="s">
+      <c r="J3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>16</v>
-      </c>
       <c r="K3" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.4">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>12345</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D4" s="3">
         <v>34680</v>
@@ -3755,30 +4201,30 @@
         <v>44487</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H4" s="2">
         <v>0</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.4">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>12346</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D5" s="3">
         <v>34681</v>
@@ -3790,30 +4236,30 @@
         <v>44488</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H5" s="2">
         <v>0</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.4">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>12347</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D6" s="3">
         <v>34682</v>
@@ -3825,30 +4271,30 @@
         <v>44489</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H6" s="2">
         <v>0</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.4">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>12348</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D7" s="3">
         <v>34683</v>
@@ -3860,19 +4306,19 @@
         <v>44490</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H7" s="2">
         <v>0</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -3880,22 +4326,22 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView zoomScale="40" zoomScaleNormal="40" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.4">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -3907,47 +4353,47 @@
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="G3" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="I3" s="2" t="s">
+      <c r="J3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="J3" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.4">
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>12345</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D4" s="3">
         <v>34680</v>
@@ -3959,27 +4405,27 @@
         <v>44487</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H4" s="2">
         <v>0</v>
       </c>
       <c r="I4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J4" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="J4" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.4">
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>12346</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D5" s="3">
         <v>34681</v>
@@ -3991,27 +4437,27 @@
         <v>44488</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H5" s="2">
         <v>0</v>
       </c>
       <c r="I5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J5" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="J5" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.4">
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>12347</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D6" s="3">
         <v>34682</v>
@@ -4023,27 +4469,27 @@
         <v>44489</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H6" s="2">
         <v>0</v>
       </c>
       <c r="I6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J6" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="J6" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.4">
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>12348</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D7" s="3">
         <v>34683</v>
@@ -4055,16 +4501,16 @@
         <v>44490</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H7" s="2">
         <v>0</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -4072,22 +4518,22 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView zoomScale="40" zoomScaleNormal="40" workbookViewId="0"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.4">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -4099,47 +4545,47 @@
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="G3" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="I3" s="2" t="s">
+      <c r="J3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="J3" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.4">
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>12345</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D4" s="3">
         <v>34680</v>
@@ -4151,27 +4597,27 @@
         <v>44487</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H4" s="2">
         <v>0</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.4">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>12346</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D5" s="3">
         <v>34681</v>
@@ -4183,27 +4629,27 @@
         <v>44488</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H5" s="2">
         <v>0</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.4">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>12347</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D6" s="3">
         <v>34682</v>
@@ -4215,27 +4661,27 @@
         <v>44489</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H6" s="2">
         <v>0</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.4">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>12348</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D7" s="3">
         <v>34683</v>
@@ -4247,16 +4693,16 @@
         <v>44490</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H7" s="2">
         <v>0</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -4264,22 +4710,22 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:Z7"/>
   <sheetViews>
     <sheetView zoomScale="40" zoomScaleNormal="40" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.4">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -4291,47 +4737,47 @@
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="G3" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="I3" s="2" t="s">
+      <c r="J3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="J3" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.4">
+    </row>
+    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>12345</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D4" s="3">
         <v>34680</v>
@@ -4343,27 +4789,27 @@
         <v>44487</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H4" s="2">
         <v>0</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.4">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>12346</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D5" s="3">
         <v>34681</v>
@@ -4375,27 +4821,27 @@
         <v>44488</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H5" s="2">
         <v>0</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.4">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>12347</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D6" s="3">
         <v>34682</v>
@@ -4407,27 +4853,27 @@
         <v>44489</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H6" s="2">
         <v>0</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.4">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>12348</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D7" s="3">
         <v>34683</v>
@@ -4439,230 +4885,19 @@
         <v>44490</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H7" s="2">
         <v>0</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="U7" s="1"/>
       <c r="Z7" s="1"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:K7"/>
-  <sheetViews>
-    <sheetView zoomScale="40" zoomScaleNormal="40" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.4"/>
-  <cols>
-    <col min="4" max="4" width="9.0546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A1" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A3" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A4" s="2">
-        <v>12345</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4" s="3">
-        <v>34680</v>
-      </c>
-      <c r="E4" s="2">
-        <v>123451</v>
-      </c>
-      <c r="F4" s="3">
-        <v>44487</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="H4" s="2">
-        <v>0</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="J4" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="K4" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A5" s="2">
-        <v>12346</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" s="3">
-        <v>34681</v>
-      </c>
-      <c r="E5" s="2">
-        <v>123452</v>
-      </c>
-      <c r="F5" s="3">
-        <v>44488</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="H5" s="2">
-        <v>0</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="J5" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="K5" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A6" s="2">
-        <v>12347</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6" s="3">
-        <v>34682</v>
-      </c>
-      <c r="E6" s="2">
-        <v>123453</v>
-      </c>
-      <c r="F6" s="3">
-        <v>44489</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="H6" s="2">
-        <v>0</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="J6" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="K6" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A7" s="2">
-        <v>12348</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D7" s="3">
-        <v>34683</v>
-      </c>
-      <c r="E7" s="2">
-        <v>123454</v>
-      </c>
-      <c r="F7" s="3">
-        <v>44490</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="H7" s="2">
-        <v>0</v>
-      </c>
-      <c r="I7" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="J7" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="K7" s="2" t="s">
-        <v>41</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>